<commit_message>
Add max length for text validation in edit-form.vue.
</commit_message>
<xml_diff>
--- a/refFiles/AGD_DBSchema_20220427_V6.xlsx
+++ b/refFiles/AGD_DBSchema_20220427_V6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="11895" windowHeight="5880"/>
   </bookViews>
   <sheets>
     <sheet name="SP_config" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10805" uniqueCount="1610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10833" uniqueCount="1610">
   <si>
     <t>聯繫原因</t>
   </si>
@@ -5932,7 +5932,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5944,7 +5944,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6:F28"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -5958,7 +5958,7 @@
     <col min="8" max="8" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.149999999999999">
+    <row r="1" spans="1:8">
       <c r="A1" s="9" t="s">
         <v>92</v>
       </c>
@@ -5991,7 +5991,9 @@
       <c r="E2" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G2" t="str">
         <f t="shared" ref="G2:G28" si="0">"using ESUN.AGD.WebApi.Application."&amp;A2&amp;";"</f>
         <v>using ESUN.AGD.WebApi.Application.User;</v>
@@ -6014,7 +6016,9 @@
       <c r="E3" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.Group;</v>
@@ -6037,7 +6041,9 @@
       <c r="E4" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.Role;</v>
@@ -6060,7 +6066,9 @@
       <c r="E5" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.Func;</v>
@@ -6083,7 +6091,9 @@
       <c r="E6" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.UserRole;</v>
@@ -6106,7 +6116,9 @@
       <c r="E7" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.RoleFunc;</v>
@@ -6129,7 +6141,9 @@
       <c r="E8" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.PcPhone;</v>
@@ -6152,7 +6166,9 @@
       <c r="E9" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.AuxCode;</v>
@@ -6175,7 +6191,9 @@
       <c r="E10" s="13" t="s">
         <v>446</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.Protocol;</v>
@@ -6198,6 +6216,9 @@
       <c r="E11" s="13" t="s">
         <v>447</v>
       </c>
+      <c r="F11" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.Code;</v>
@@ -6220,7 +6241,9 @@
       <c r="E12" s="13" t="s">
         <v>459</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.PhoneBook;</v>
@@ -6243,7 +6266,9 @@
       <c r="E13" s="13" t="s">
         <v>449</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.Reason;</v>
@@ -6266,7 +6291,9 @@
       <c r="E14" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.ReasonIvr;</v>
@@ -6289,7 +6316,9 @@
       <c r="E15" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.ReasonTxn;</v>
@@ -6312,7 +6341,9 @@
       <c r="E16" s="13" t="s">
         <v>1515</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G16" t="str">
         <f t="shared" ref="G16" si="2">"using ESUN.AGD.WebApi.Application."&amp;A16&amp;";"</f>
         <v>using ESUN.AGD.WebApi.Application.CipCode;</v>
@@ -6335,7 +6366,9 @@
       <c r="E17" s="13" t="s">
         <v>1105</v>
       </c>
-      <c r="F17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.UserShift;</v>
@@ -6358,7 +6391,9 @@
       <c r="E18" s="13" t="s">
         <v>462</v>
       </c>
-      <c r="F18" s="6"/>
+      <c r="F18" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.NotificationTemplate;</v>
@@ -6382,7 +6417,9 @@
       <c r="E19" s="13" t="s">
         <v>463</v>
       </c>
-      <c r="F19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.MessageSheet;</v>
@@ -6406,7 +6443,9 @@
       <c r="E20" s="13" t="s">
         <v>454</v>
       </c>
-      <c r="F20" s="6"/>
+      <c r="F20" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.Message;</v>
@@ -6430,7 +6469,9 @@
       <c r="E21" s="13" t="s">
         <v>464</v>
       </c>
-      <c r="F21" s="6"/>
+      <c r="F21" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.MessageTemplate;</v>
@@ -6454,7 +6495,9 @@
       <c r="E22" s="13" t="s">
         <v>465</v>
       </c>
-      <c r="F22" s="6"/>
+      <c r="F22" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G22" t="str">
         <f t="shared" ref="G22:G24" si="4">"using ESUN.AGD.WebApi.Application."&amp;A22&amp;";"</f>
         <v>using ESUN.AGD.WebApi.Application.Txn;</v>
@@ -6478,7 +6521,9 @@
       <c r="E23" s="13" t="s">
         <v>1496</v>
       </c>
-      <c r="F23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G23" t="str">
         <f t="shared" si="4"/>
         <v>using ESUN.AGD.WebApi.Application.AccidentFormTemplate;</v>
@@ -6502,7 +6547,9 @@
       <c r="E24" s="13" t="s">
         <v>1469</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G24" t="str">
         <f t="shared" si="4"/>
         <v>using ESUN.AGD.WebApi.Application.AccidentScript;</v>
@@ -6526,7 +6573,9 @@
       <c r="E25" s="13" t="s">
         <v>1429</v>
       </c>
-      <c r="F25" s="6"/>
+      <c r="F25" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.ZipCity;</v>
@@ -6550,7 +6599,9 @@
       <c r="E26" s="13" t="s">
         <v>1431</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.ZipRoad;</v>
@@ -6574,7 +6625,9 @@
       <c r="E27" s="13" t="s">
         <v>456</v>
       </c>
-      <c r="F27" s="6"/>
+      <c r="F27" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.Marketing;</v>
@@ -6598,7 +6651,9 @@
       <c r="E28" s="13" t="s">
         <v>466</v>
       </c>
-      <c r="F28" s="6"/>
+      <c r="F28" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
         <v>using ESUN.AGD.WebApi.Application.MarketingActionCode;</v>
@@ -6647,7 +6702,9 @@
       <c r="E30" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="F30" s="6"/>
+      <c r="F30" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="G30" t="str">
         <f>"using ESUN.AGD.WebApi.Application."&amp;A30&amp;";"</f>
         <v>using ESUN.AGD.WebApi.Application.SysConfig;</v>
@@ -16700,7 +16757,7 @@
     <col min="25" max="25" width="12.25" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="16.149999999999999">
+    <row r="1" spans="1:25">
       <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
@@ -37789,7 +37846,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16.149999999999999">
+    <row r="3" spans="1:9">
       <c r="A3" s="19" t="s">
         <v>155</v>
       </c>
@@ -38149,7 +38206,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.149999999999999">
+    <row r="12" spans="1:9">
       <c r="A12" s="19" t="s">
         <v>165</v>
       </c>
@@ -42477,7 +42534,7 @@
     <col min="14" max="16384" width="8.875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16.149999999999999">
+    <row r="1" spans="1:19">
       <c r="A1" s="19" t="s">
         <v>343</v>
       </c>

</xml_diff>